<commit_message>
Update matriz de trazabilidad
</commit_message>
<xml_diff>
--- a/Documentacion/Matriz.xlsx
+++ b/Documentacion/Matriz.xlsx
@@ -94,8 +94,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="165" formatCode="General"/>
   </numFmts>
   <fonts count="6">
     <font>
@@ -134,7 +135,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="14">
+  <fills count="15">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -192,7 +193,7 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFC4BD97"/>
-        <bgColor rgb="FFC3D69B"/>
+        <bgColor rgb="FFB2B2B2"/>
       </patternFill>
     </fill>
     <fill>
@@ -204,6 +205,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFE6B9B8"/>
+        <bgColor rgb="FFC4BD97"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFB2B2B2"/>
         <bgColor rgb="FFC4BD97"/>
       </patternFill>
     </fill>
@@ -269,7 +276,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="25">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -354,7 +361,15 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="13" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="13" borderId="3" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="14" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -420,7 +435,7 @@
       <rgbColor rgb="FFFF9900"/>
       <rgbColor rgb="FFFF6600"/>
       <rgbColor rgb="FF666699"/>
-      <rgbColor rgb="FF969696"/>
+      <rgbColor rgb="FFB2B2B2"/>
       <rgbColor rgb="FF003366"/>
       <rgbColor rgb="FF339966"/>
       <rgbColor rgb="FF003300"/>
@@ -441,13 +456,13 @@
   </sheetPr>
   <dimension ref="B4:CW145"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="AR64" colorId="64" zoomScale="28" zoomScaleNormal="28" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="CJ150" activeCellId="0" sqref="CJ150"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D108" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H128" activeCellId="0" sqref="H128"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.5390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="4.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="4.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="4.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="3.86"/>
     <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="6" min="6" style="0" width="3.14"/>
@@ -458,7 +473,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="4.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="4.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="5.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="5.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="4.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="18" style="0" width="4.28"/>
@@ -469,38 +484,38 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="24" min="24" style="0" width="6"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="25" style="0" width="5.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="26" style="0" width="6"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="27" min="27" style="0" width="5.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="27" min="27" style="0" width="5.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="33" min="28" style="0" width="5.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="34" min="34" style="0" width="5.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="35" min="35" style="0" width="5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="36" min="36" style="0" width="4.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="37" min="37" style="0" width="5.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="38" min="38" style="0" width="4.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="37" min="37" style="0" width="5.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="38" min="38" style="0" width="4.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="39" min="39" style="0" width="5.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="40" min="40" style="0" width="5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="41" min="41" style="0" width="5.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="42" min="42" style="0" width="5.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="43" min="43" style="0" width="4.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="43" min="43" style="0" width="4.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="44" min="44" style="0" width="5.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="45" min="45" style="0" width="5.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="46" min="46" style="0" width="4.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="47" min="47" style="0" width="5.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="48" min="48" style="0" width="5.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="48" min="48" style="0" width="5.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="49" min="49" style="0" width="5.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="50" min="50" style="0" width="6.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="51" min="51" style="0" width="5.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="52" min="52" style="0" width="6.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="53" min="53" style="0" width="5.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="53" min="53" style="0" width="5.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="54" min="54" style="0" width="4.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="55" min="55" style="0" width="5.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="56" min="56" style="0" width="6.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="57" min="57" style="0" width="5.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="58" min="58" style="0" width="5.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="58" min="58" style="0" width="5.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="61" min="59" style="0" width="5.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="62" min="62" style="0" width="4.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="64" min="63" style="0" width="5.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="65" min="65" style="0" width="5.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="67" min="66" style="0" width="4.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="67" min="66" style="0" width="4.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="68" min="68" style="0" width="5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="69" min="69" style="0" width="5.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="70" min="70" style="0" width="5.57"/>
@@ -508,7 +523,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="72" min="72" style="0" width="5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="73" min="73" style="0" width="5.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="74" min="74" style="0" width="5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="75" min="75" style="0" width="5.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="75" min="75" style="0" width="5.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="76" min="76" style="0" width="4.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="77" min="77" style="0" width="5.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="78" min="78" style="0" width="5.43"/>
@@ -516,19 +531,19 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="81" min="81" style="0" width="5.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="82" min="82" style="0" width="5.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="83" min="83" style="0" width="5.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="84" min="84" style="0" width="5.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="84" min="84" style="0" width="5.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="85" min="85" style="0" width="5.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="87" min="86" style="0" width="5.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="88" min="88" style="0" width="5.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="89" min="89" style="0" width="5.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="89" min="89" style="0" width="5.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="90" min="90" style="0" width="5.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="91" min="91" style="0" width="6.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="92" min="92" style="0" width="6.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="93" min="93" style="0" width="5.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="93" min="93" style="0" width="5.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="94" min="94" style="0" width="5.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="96" min="95" style="0" width="6"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="97" min="97" style="0" width="6.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="98" min="98" style="0" width="5.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="98" min="98" style="0" width="5.51"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="99" min="99" style="0" width="6.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="100" min="100" style="0" width="5.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="101" min="101" style="0" width="6.28"/>
@@ -10057,8 +10072,8 @@
       <c r="BX105" s="12"/>
       <c r="BY105" s="12"/>
       <c r="BZ105" s="12"/>
-      <c r="CA105" s="12"/>
-      <c r="CB105" s="12"/>
+      <c r="CA105" s="11"/>
+      <c r="CB105" s="11"/>
       <c r="CC105" s="12"/>
       <c r="CD105" s="12"/>
       <c r="CE105" s="12"/>
@@ -10471,8 +10486,8 @@
       <c r="BZ109" s="12"/>
       <c r="CA109" s="12"/>
       <c r="CB109" s="12"/>
-      <c r="CC109" s="12"/>
-      <c r="CD109" s="12"/>
+      <c r="CC109" s="11"/>
+      <c r="CD109" s="11"/>
       <c r="CE109" s="12"/>
       <c r="CF109" s="12"/>
       <c r="CG109" s="12"/>
@@ -10580,8 +10595,8 @@
       <c r="CF110" s="12"/>
       <c r="CG110" s="12"/>
       <c r="CH110" s="12"/>
-      <c r="CI110" s="12"/>
-      <c r="CJ110" s="12"/>
+      <c r="CI110" s="11"/>
+      <c r="CJ110" s="11"/>
       <c r="CK110" s="12"/>
       <c r="CL110" s="12"/>
       <c r="CM110" s="12"/>
@@ -10681,8 +10696,8 @@
       <c r="CD111" s="12"/>
       <c r="CE111" s="12"/>
       <c r="CF111" s="12"/>
-      <c r="CG111" s="12"/>
-      <c r="CH111" s="12"/>
+      <c r="CG111" s="11"/>
+      <c r="CH111" s="11"/>
       <c r="CI111" s="12"/>
       <c r="CJ111" s="12"/>
       <c r="CK111" s="12"/>
@@ -10782,8 +10797,8 @@
       <c r="CB112" s="12"/>
       <c r="CC112" s="12"/>
       <c r="CD112" s="12"/>
-      <c r="CE112" s="12"/>
-      <c r="CF112" s="12"/>
+      <c r="CE112" s="11"/>
+      <c r="CF112" s="11"/>
       <c r="CG112" s="12"/>
       <c r="CH112" s="12"/>
       <c r="CI112" s="12"/>
@@ -10891,9 +10906,9 @@
       <c r="CH113" s="12"/>
       <c r="CI113" s="12"/>
       <c r="CJ113" s="12"/>
-      <c r="CK113" s="12"/>
+      <c r="CK113" s="11"/>
       <c r="CL113" s="12"/>
-      <c r="CM113" s="12"/>
+      <c r="CM113" s="11"/>
       <c r="CN113" s="12"/>
       <c r="CO113" s="12"/>
       <c r="CP113" s="12"/>
@@ -10995,8 +11010,8 @@
       <c r="CI114" s="12"/>
       <c r="CJ114" s="12"/>
       <c r="CK114" s="12"/>
-      <c r="CL114" s="12"/>
-      <c r="CM114" s="12"/>
+      <c r="CL114" s="11"/>
+      <c r="CM114" s="11"/>
       <c r="CN114" s="12"/>
       <c r="CO114" s="12"/>
       <c r="CP114" s="12"/>
@@ -11100,9 +11115,9 @@
       <c r="CK115" s="12"/>
       <c r="CL115" s="12"/>
       <c r="CM115" s="12"/>
-      <c r="CN115" s="12"/>
+      <c r="CN115" s="11"/>
       <c r="CO115" s="12"/>
-      <c r="CP115" s="12"/>
+      <c r="CP115" s="11"/>
       <c r="CQ115" s="12"/>
       <c r="CR115" s="12"/>
       <c r="CS115" s="12"/>
@@ -11204,8 +11219,8 @@
       <c r="CL116" s="12"/>
       <c r="CM116" s="12"/>
       <c r="CN116" s="12"/>
-      <c r="CO116" s="12"/>
-      <c r="CP116" s="12"/>
+      <c r="CO116" s="11"/>
+      <c r="CP116" s="11"/>
       <c r="CQ116" s="12"/>
       <c r="CR116" s="12"/>
       <c r="CS116" s="12"/>
@@ -11309,7 +11324,7 @@
       <c r="CN117" s="12"/>
       <c r="CO117" s="12"/>
       <c r="CP117" s="12"/>
-      <c r="CQ117" s="12"/>
+      <c r="CQ117" s="11"/>
       <c r="CR117" s="12"/>
       <c r="CS117" s="12"/>
       <c r="CT117" s="12"/>
@@ -11412,8 +11427,8 @@
       <c r="CN118" s="12"/>
       <c r="CO118" s="12"/>
       <c r="CP118" s="12"/>
-      <c r="CQ118" s="12"/>
-      <c r="CR118" s="12"/>
+      <c r="CQ118" s="21"/>
+      <c r="CR118" s="11"/>
       <c r="CS118" s="12"/>
       <c r="CT118" s="12"/>
       <c r="CU118" s="12"/>
@@ -11517,7 +11532,7 @@
       <c r="CP119" s="12"/>
       <c r="CQ119" s="12"/>
       <c r="CR119" s="12"/>
-      <c r="CS119" s="12"/>
+      <c r="CS119" s="11"/>
       <c r="CT119" s="12"/>
       <c r="CU119" s="12"/>
       <c r="CV119" s="12"/>
@@ -11621,7 +11636,7 @@
       <c r="CQ120" s="12"/>
       <c r="CR120" s="12"/>
       <c r="CS120" s="12"/>
-      <c r="CT120" s="12"/>
+      <c r="CT120" s="11"/>
       <c r="CU120" s="12"/>
       <c r="CV120" s="12"/>
       <c r="CW120" s="12"/>
@@ -11827,7 +11842,7 @@
       <c r="CQ122" s="12"/>
       <c r="CR122" s="12"/>
       <c r="CS122" s="12"/>
-      <c r="CT122" s="12"/>
+      <c r="CT122" s="11"/>
       <c r="CU122" s="12"/>
       <c r="CV122" s="12"/>
       <c r="CW122" s="12"/>
@@ -11931,7 +11946,7 @@
       <c r="CR123" s="12"/>
       <c r="CS123" s="12"/>
       <c r="CT123" s="12"/>
-      <c r="CU123" s="12"/>
+      <c r="CU123" s="11"/>
       <c r="CV123" s="12"/>
       <c r="CW123" s="12"/>
     </row>
@@ -12136,12 +12151,12 @@
       <c r="CQ125" s="12"/>
       <c r="CR125" s="12"/>
       <c r="CS125" s="12"/>
-      <c r="CT125" s="12"/>
-      <c r="CU125" s="12"/>
+      <c r="CT125" s="11"/>
+      <c r="CU125" s="11"/>
       <c r="CV125" s="12"/>
       <c r="CW125" s="12"/>
     </row>
-    <row r="126" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="126" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C126" s="7"/>
       <c r="D126" s="8"/>
       <c r="E126" s="9" t="n">
@@ -12241,10 +12256,10 @@
       <c r="CS126" s="12"/>
       <c r="CT126" s="12"/>
       <c r="CU126" s="12"/>
-      <c r="CV126" s="12"/>
-      <c r="CW126" s="12"/>
-    </row>
-    <row r="127" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="CV126" s="11"/>
+      <c r="CW126" s="11"/>
+    </row>
+    <row r="127" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C127" s="7"/>
       <c r="D127" s="8"/>
       <c r="E127" s="9" t="n">
@@ -12350,7 +12365,7 @@
     <row r="128" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C128" s="7"/>
       <c r="D128" s="8"/>
-      <c r="E128" s="9" t="n">
+      <c r="E128" s="22" t="n">
         <f aca="false">E127+1</f>
         <v>87</v>
       </c>
@@ -12450,10 +12465,10 @@
       <c r="CV128" s="12"/>
       <c r="CW128" s="12"/>
     </row>
-    <row r="129" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="129" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C129" s="7"/>
       <c r="D129" s="8"/>
-      <c r="E129" s="9" t="n">
+      <c r="E129" s="22" t="n">
         <f aca="false">E128+1</f>
         <v>88</v>
       </c>
@@ -12553,10 +12568,10 @@
       <c r="CV129" s="12"/>
       <c r="CW129" s="12"/>
     </row>
-    <row r="130" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="130" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C130" s="7"/>
       <c r="D130" s="8"/>
-      <c r="E130" s="9" t="n">
+      <c r="E130" s="22" t="n">
         <f aca="false">E129+1</f>
         <v>89</v>
       </c>
@@ -12656,10 +12671,10 @@
       <c r="CV130" s="12"/>
       <c r="CW130" s="12"/>
     </row>
-    <row r="131" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="131" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C131" s="7"/>
       <c r="D131" s="8"/>
-      <c r="E131" s="9" t="n">
+      <c r="E131" s="22" t="n">
         <f aca="false">E130+1</f>
         <v>90</v>
       </c>
@@ -12761,7 +12776,7 @@
     </row>
     <row r="132" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C132" s="7"/>
-      <c r="D132" s="21" t="s">
+      <c r="D132" s="23" t="s">
         <v>21</v>
       </c>
       <c r="E132" s="10" t="n">
@@ -12865,7 +12880,7 @@
     </row>
     <row r="133" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C133" s="7"/>
-      <c r="D133" s="21"/>
+      <c r="D133" s="23"/>
       <c r="E133" s="10" t="n">
         <f aca="false">E132+1</f>
         <v>2</v>
@@ -12968,7 +12983,7 @@
     </row>
     <row r="134" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C134" s="7"/>
-      <c r="D134" s="21"/>
+      <c r="D134" s="23"/>
       <c r="E134" s="10" t="n">
         <f aca="false">E133+1</f>
         <v>3</v>
@@ -13071,7 +13086,7 @@
     </row>
     <row r="135" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C135" s="7"/>
-      <c r="D135" s="21"/>
+      <c r="D135" s="23"/>
       <c r="E135" s="10" t="n">
         <f aca="false">E134+1</f>
         <v>4</v>
@@ -13174,7 +13189,7 @@
     </row>
     <row r="136" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C136" s="7"/>
-      <c r="D136" s="21"/>
+      <c r="D136" s="23"/>
       <c r="E136" s="9" t="n">
         <f aca="false">E135+1</f>
         <v>5</v>
@@ -13277,23 +13292,23 @@
     </row>
     <row r="137" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C137" s="3"/>
-      <c r="D137" s="22"/>
+      <c r="D137" s="24"/>
     </row>
     <row r="138" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C138" s="3"/>
-      <c r="D138" s="22"/>
+      <c r="D138" s="24"/>
     </row>
     <row r="139" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C139" s="3"/>
-      <c r="D139" s="22"/>
+      <c r="D139" s="24"/>
     </row>
     <row r="140" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C140" s="3"/>
-      <c r="D140" s="22"/>
+      <c r="D140" s="24"/>
     </row>
     <row r="141" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C141" s="3"/>
-      <c r="D141" s="22"/>
+      <c r="D141" s="24"/>
     </row>
     <row r="142" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C142" s="3"/>
@@ -13331,11 +13346,11 @@
   </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="28" zoomScaleNormal="28" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.5390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
@@ -13354,11 +13369,11 @@
   </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="28" zoomScaleNormal="28" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.5390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>

<commit_message>
Update Tabla de CasosdePrueba&Matriz - Branch main
</commit_message>
<xml_diff>
--- a/Documentacion/Matriz.xlsx
+++ b/Documentacion/Matriz.xlsx
@@ -94,8 +94,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="165" formatCode="General"/>
   </numFmts>
   <fonts count="6">
     <font>
@@ -134,7 +135,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="14">
+  <fills count="15">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -192,7 +193,7 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFC4BD97"/>
-        <bgColor rgb="FFC3D69B"/>
+        <bgColor rgb="FFB2B2B2"/>
       </patternFill>
     </fill>
     <fill>
@@ -204,6 +205,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFE6B9B8"/>
+        <bgColor rgb="FFC4BD97"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFB2B2B2"/>
         <bgColor rgb="FFC4BD97"/>
       </patternFill>
     </fill>
@@ -269,7 +276,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="25">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -354,7 +361,15 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="13" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="13" borderId="3" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="14" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -420,7 +435,7 @@
       <rgbColor rgb="FFFF9900"/>
       <rgbColor rgb="FFFF6600"/>
       <rgbColor rgb="FF666699"/>
-      <rgbColor rgb="FF969696"/>
+      <rgbColor rgb="FFB2B2B2"/>
       <rgbColor rgb="FF003366"/>
       <rgbColor rgb="FF339966"/>
       <rgbColor rgb="FF003300"/>
@@ -441,13 +456,13 @@
   </sheetPr>
   <dimension ref="B4:CW145"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="AR64" colorId="64" zoomScale="28" zoomScaleNormal="28" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="CJ150" activeCellId="0" sqref="CJ150"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D108" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H128" activeCellId="0" sqref="H128"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.5390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="4.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="4.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="4.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="3.86"/>
     <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="6" min="6" style="0" width="3.14"/>
@@ -458,7 +473,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="4.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="4.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="5.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="5.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="4.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="18" style="0" width="4.28"/>
@@ -469,38 +484,38 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="24" min="24" style="0" width="6"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="25" style="0" width="5.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="26" style="0" width="6"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="27" min="27" style="0" width="5.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="27" min="27" style="0" width="5.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="33" min="28" style="0" width="5.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="34" min="34" style="0" width="5.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="35" min="35" style="0" width="5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="36" min="36" style="0" width="4.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="37" min="37" style="0" width="5.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="38" min="38" style="0" width="4.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="37" min="37" style="0" width="5.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="38" min="38" style="0" width="4.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="39" min="39" style="0" width="5.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="40" min="40" style="0" width="5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="41" min="41" style="0" width="5.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="42" min="42" style="0" width="5.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="43" min="43" style="0" width="4.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="43" min="43" style="0" width="4.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="44" min="44" style="0" width="5.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="45" min="45" style="0" width="5.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="46" min="46" style="0" width="4.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="47" min="47" style="0" width="5.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="48" min="48" style="0" width="5.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="48" min="48" style="0" width="5.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="49" min="49" style="0" width="5.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="50" min="50" style="0" width="6.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="51" min="51" style="0" width="5.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="52" min="52" style="0" width="6.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="53" min="53" style="0" width="5.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="53" min="53" style="0" width="5.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="54" min="54" style="0" width="4.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="55" min="55" style="0" width="5.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="56" min="56" style="0" width="6.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="57" min="57" style="0" width="5.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="58" min="58" style="0" width="5.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="58" min="58" style="0" width="5.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="61" min="59" style="0" width="5.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="62" min="62" style="0" width="4.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="64" min="63" style="0" width="5.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="65" min="65" style="0" width="5.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="67" min="66" style="0" width="4.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="67" min="66" style="0" width="4.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="68" min="68" style="0" width="5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="69" min="69" style="0" width="5.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="70" min="70" style="0" width="5.57"/>
@@ -508,7 +523,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="72" min="72" style="0" width="5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="73" min="73" style="0" width="5.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="74" min="74" style="0" width="5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="75" min="75" style="0" width="5.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="75" min="75" style="0" width="5.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="76" min="76" style="0" width="4.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="77" min="77" style="0" width="5.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="78" min="78" style="0" width="5.43"/>
@@ -516,19 +531,19 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="81" min="81" style="0" width="5.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="82" min="82" style="0" width="5.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="83" min="83" style="0" width="5.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="84" min="84" style="0" width="5.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="84" min="84" style="0" width="5.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="85" min="85" style="0" width="5.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="87" min="86" style="0" width="5.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="88" min="88" style="0" width="5.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="89" min="89" style="0" width="5.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="89" min="89" style="0" width="5.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="90" min="90" style="0" width="5.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="91" min="91" style="0" width="6.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="92" min="92" style="0" width="6.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="93" min="93" style="0" width="5.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="93" min="93" style="0" width="5.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="94" min="94" style="0" width="5.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="96" min="95" style="0" width="6"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="97" min="97" style="0" width="6.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="98" min="98" style="0" width="5.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="98" min="98" style="0" width="5.51"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="99" min="99" style="0" width="6.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="100" min="100" style="0" width="5.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="101" min="101" style="0" width="6.28"/>
@@ -10057,8 +10072,8 @@
       <c r="BX105" s="12"/>
       <c r="BY105" s="12"/>
       <c r="BZ105" s="12"/>
-      <c r="CA105" s="12"/>
-      <c r="CB105" s="12"/>
+      <c r="CA105" s="11"/>
+      <c r="CB105" s="11"/>
       <c r="CC105" s="12"/>
       <c r="CD105" s="12"/>
       <c r="CE105" s="12"/>
@@ -10471,8 +10486,8 @@
       <c r="BZ109" s="12"/>
       <c r="CA109" s="12"/>
       <c r="CB109" s="12"/>
-      <c r="CC109" s="12"/>
-      <c r="CD109" s="12"/>
+      <c r="CC109" s="11"/>
+      <c r="CD109" s="11"/>
       <c r="CE109" s="12"/>
       <c r="CF109" s="12"/>
       <c r="CG109" s="12"/>
@@ -10580,8 +10595,8 @@
       <c r="CF110" s="12"/>
       <c r="CG110" s="12"/>
       <c r="CH110" s="12"/>
-      <c r="CI110" s="12"/>
-      <c r="CJ110" s="12"/>
+      <c r="CI110" s="11"/>
+      <c r="CJ110" s="11"/>
       <c r="CK110" s="12"/>
       <c r="CL110" s="12"/>
       <c r="CM110" s="12"/>
@@ -10681,8 +10696,8 @@
       <c r="CD111" s="12"/>
       <c r="CE111" s="12"/>
       <c r="CF111" s="12"/>
-      <c r="CG111" s="12"/>
-      <c r="CH111" s="12"/>
+      <c r="CG111" s="11"/>
+      <c r="CH111" s="11"/>
       <c r="CI111" s="12"/>
       <c r="CJ111" s="12"/>
       <c r="CK111" s="12"/>
@@ -10782,8 +10797,8 @@
       <c r="CB112" s="12"/>
       <c r="CC112" s="12"/>
       <c r="CD112" s="12"/>
-      <c r="CE112" s="12"/>
-      <c r="CF112" s="12"/>
+      <c r="CE112" s="11"/>
+      <c r="CF112" s="11"/>
       <c r="CG112" s="12"/>
       <c r="CH112" s="12"/>
       <c r="CI112" s="12"/>
@@ -10891,9 +10906,9 @@
       <c r="CH113" s="12"/>
       <c r="CI113" s="12"/>
       <c r="CJ113" s="12"/>
-      <c r="CK113" s="12"/>
+      <c r="CK113" s="11"/>
       <c r="CL113" s="12"/>
-      <c r="CM113" s="12"/>
+      <c r="CM113" s="11"/>
       <c r="CN113" s="12"/>
       <c r="CO113" s="12"/>
       <c r="CP113" s="12"/>
@@ -10995,8 +11010,8 @@
       <c r="CI114" s="12"/>
       <c r="CJ114" s="12"/>
       <c r="CK114" s="12"/>
-      <c r="CL114" s="12"/>
-      <c r="CM114" s="12"/>
+      <c r="CL114" s="11"/>
+      <c r="CM114" s="11"/>
       <c r="CN114" s="12"/>
       <c r="CO114" s="12"/>
       <c r="CP114" s="12"/>
@@ -11100,9 +11115,9 @@
       <c r="CK115" s="12"/>
       <c r="CL115" s="12"/>
       <c r="CM115" s="12"/>
-      <c r="CN115" s="12"/>
+      <c r="CN115" s="11"/>
       <c r="CO115" s="12"/>
-      <c r="CP115" s="12"/>
+      <c r="CP115" s="11"/>
       <c r="CQ115" s="12"/>
       <c r="CR115" s="12"/>
       <c r="CS115" s="12"/>
@@ -11204,8 +11219,8 @@
       <c r="CL116" s="12"/>
       <c r="CM116" s="12"/>
       <c r="CN116" s="12"/>
-      <c r="CO116" s="12"/>
-      <c r="CP116" s="12"/>
+      <c r="CO116" s="11"/>
+      <c r="CP116" s="11"/>
       <c r="CQ116" s="12"/>
       <c r="CR116" s="12"/>
       <c r="CS116" s="12"/>
@@ -11309,7 +11324,7 @@
       <c r="CN117" s="12"/>
       <c r="CO117" s="12"/>
       <c r="CP117" s="12"/>
-      <c r="CQ117" s="12"/>
+      <c r="CQ117" s="11"/>
       <c r="CR117" s="12"/>
       <c r="CS117" s="12"/>
       <c r="CT117" s="12"/>
@@ -11412,8 +11427,8 @@
       <c r="CN118" s="12"/>
       <c r="CO118" s="12"/>
       <c r="CP118" s="12"/>
-      <c r="CQ118" s="12"/>
-      <c r="CR118" s="12"/>
+      <c r="CQ118" s="21"/>
+      <c r="CR118" s="11"/>
       <c r="CS118" s="12"/>
       <c r="CT118" s="12"/>
       <c r="CU118" s="12"/>
@@ -11517,7 +11532,7 @@
       <c r="CP119" s="12"/>
       <c r="CQ119" s="12"/>
       <c r="CR119" s="12"/>
-      <c r="CS119" s="12"/>
+      <c r="CS119" s="11"/>
       <c r="CT119" s="12"/>
       <c r="CU119" s="12"/>
       <c r="CV119" s="12"/>
@@ -11621,7 +11636,7 @@
       <c r="CQ120" s="12"/>
       <c r="CR120" s="12"/>
       <c r="CS120" s="12"/>
-      <c r="CT120" s="12"/>
+      <c r="CT120" s="11"/>
       <c r="CU120" s="12"/>
       <c r="CV120" s="12"/>
       <c r="CW120" s="12"/>
@@ -11827,7 +11842,7 @@
       <c r="CQ122" s="12"/>
       <c r="CR122" s="12"/>
       <c r="CS122" s="12"/>
-      <c r="CT122" s="12"/>
+      <c r="CT122" s="11"/>
       <c r="CU122" s="12"/>
       <c r="CV122" s="12"/>
       <c r="CW122" s="12"/>
@@ -11931,7 +11946,7 @@
       <c r="CR123" s="12"/>
       <c r="CS123" s="12"/>
       <c r="CT123" s="12"/>
-      <c r="CU123" s="12"/>
+      <c r="CU123" s="11"/>
       <c r="CV123" s="12"/>
       <c r="CW123" s="12"/>
     </row>
@@ -12136,12 +12151,12 @@
       <c r="CQ125" s="12"/>
       <c r="CR125" s="12"/>
       <c r="CS125" s="12"/>
-      <c r="CT125" s="12"/>
-      <c r="CU125" s="12"/>
+      <c r="CT125" s="11"/>
+      <c r="CU125" s="11"/>
       <c r="CV125" s="12"/>
       <c r="CW125" s="12"/>
     </row>
-    <row r="126" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="126" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C126" s="7"/>
       <c r="D126" s="8"/>
       <c r="E126" s="9" t="n">
@@ -12241,10 +12256,10 @@
       <c r="CS126" s="12"/>
       <c r="CT126" s="12"/>
       <c r="CU126" s="12"/>
-      <c r="CV126" s="12"/>
-      <c r="CW126" s="12"/>
-    </row>
-    <row r="127" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="CV126" s="11"/>
+      <c r="CW126" s="11"/>
+    </row>
+    <row r="127" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C127" s="7"/>
       <c r="D127" s="8"/>
       <c r="E127" s="9" t="n">
@@ -12350,7 +12365,7 @@
     <row r="128" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C128" s="7"/>
       <c r="D128" s="8"/>
-      <c r="E128" s="9" t="n">
+      <c r="E128" s="22" t="n">
         <f aca="false">E127+1</f>
         <v>87</v>
       </c>
@@ -12450,10 +12465,10 @@
       <c r="CV128" s="12"/>
       <c r="CW128" s="12"/>
     </row>
-    <row r="129" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="129" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C129" s="7"/>
       <c r="D129" s="8"/>
-      <c r="E129" s="9" t="n">
+      <c r="E129" s="22" t="n">
         <f aca="false">E128+1</f>
         <v>88</v>
       </c>
@@ -12553,10 +12568,10 @@
       <c r="CV129" s="12"/>
       <c r="CW129" s="12"/>
     </row>
-    <row r="130" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="130" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C130" s="7"/>
       <c r="D130" s="8"/>
-      <c r="E130" s="9" t="n">
+      <c r="E130" s="22" t="n">
         <f aca="false">E129+1</f>
         <v>89</v>
       </c>
@@ -12656,10 +12671,10 @@
       <c r="CV130" s="12"/>
       <c r="CW130" s="12"/>
     </row>
-    <row r="131" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="131" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C131" s="7"/>
       <c r="D131" s="8"/>
-      <c r="E131" s="9" t="n">
+      <c r="E131" s="22" t="n">
         <f aca="false">E130+1</f>
         <v>90</v>
       </c>
@@ -12761,7 +12776,7 @@
     </row>
     <row r="132" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C132" s="7"/>
-      <c r="D132" s="21" t="s">
+      <c r="D132" s="23" t="s">
         <v>21</v>
       </c>
       <c r="E132" s="10" t="n">
@@ -12865,7 +12880,7 @@
     </row>
     <row r="133" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C133" s="7"/>
-      <c r="D133" s="21"/>
+      <c r="D133" s="23"/>
       <c r="E133" s="10" t="n">
         <f aca="false">E132+1</f>
         <v>2</v>
@@ -12968,7 +12983,7 @@
     </row>
     <row r="134" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C134" s="7"/>
-      <c r="D134" s="21"/>
+      <c r="D134" s="23"/>
       <c r="E134" s="10" t="n">
         <f aca="false">E133+1</f>
         <v>3</v>
@@ -13071,7 +13086,7 @@
     </row>
     <row r="135" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C135" s="7"/>
-      <c r="D135" s="21"/>
+      <c r="D135" s="23"/>
       <c r="E135" s="10" t="n">
         <f aca="false">E134+1</f>
         <v>4</v>
@@ -13174,7 +13189,7 @@
     </row>
     <row r="136" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C136" s="7"/>
-      <c r="D136" s="21"/>
+      <c r="D136" s="23"/>
       <c r="E136" s="9" t="n">
         <f aca="false">E135+1</f>
         <v>5</v>
@@ -13277,23 +13292,23 @@
     </row>
     <row r="137" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C137" s="3"/>
-      <c r="D137" s="22"/>
+      <c r="D137" s="24"/>
     </row>
     <row r="138" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C138" s="3"/>
-      <c r="D138" s="22"/>
+      <c r="D138" s="24"/>
     </row>
     <row r="139" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C139" s="3"/>
-      <c r="D139" s="22"/>
+      <c r="D139" s="24"/>
     </row>
     <row r="140" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C140" s="3"/>
-      <c r="D140" s="22"/>
+      <c r="D140" s="24"/>
     </row>
     <row r="141" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C141" s="3"/>
-      <c r="D141" s="22"/>
+      <c r="D141" s="24"/>
     </row>
     <row r="142" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C142" s="3"/>
@@ -13331,11 +13346,11 @@
   </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="28" zoomScaleNormal="28" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.5390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
@@ -13354,11 +13369,11 @@
   </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="28" zoomScaleNormal="28" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.5390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>